<commit_message>
Task 1 almost finished, missing rmd
</commit_message>
<xml_diff>
--- a/nodes.xlsx
+++ b/nodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theib\OneDrive\Documentos\Network_Analysis_Kaggle_Star_Wars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF42867-094C-49FE-BE48-239118B6FF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C3B4C0-7792-4C8B-8A26-DB16DF478C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="132">
   <si>
     <t>name</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>TEY HOW</t>
-  </si>
-  <si>
-    <t>#191970</t>
   </si>
   <si>
     <t>EMPEROR</t>
@@ -808,7 +805,7 @@
   <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E117" sqref="E117"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,10 +1000,10 @@
         <v>52</v>
       </c>
       <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,7 +1017,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,7 +1031,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,10 +1042,10 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
         <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,7 +1059,7 @@
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1076,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1087,10 +1084,10 @@
         <v>75</v>
       </c>
       <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
         <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,7 +1101,7 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,7 +1115,7 @@
         <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,7 +1129,7 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,7 +1143,7 @@
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,7 +1157,7 @@
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,10 +1168,10 @@
         <v>151</v>
       </c>
       <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
         <v>38</v>
-      </c>
-      <c r="D26" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,7 +1185,7 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,7 +1199,7 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,7 +1213,7 @@
         <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,7 +1227,7 @@
         <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,7 +1255,7 @@
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,7 +1269,7 @@
         <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,7 +1283,7 @@
         <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,7 +1297,7 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,10 +1308,10 @@
         <v>46</v>
       </c>
       <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
         <v>49</v>
-      </c>
-      <c r="D36" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,7 +1325,7 @@
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,7 +1339,7 @@
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,7 +1353,7 @@
         <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,7 +1367,7 @@
         <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,7 +1381,7 @@
         <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,7 +1395,7 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,7 +1409,7 @@
         <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,7 +1423,7 @@
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,7 +1437,7 @@
         <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,7 +1451,7 @@
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1468,7 +1465,7 @@
         <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,7 +1479,7 @@
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1496,7 +1493,7 @@
         <v>14</v>
       </c>
       <c r="D49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,7 +1507,7 @@
         <v>14</v>
       </c>
       <c r="D50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1524,7 +1521,7 @@
         <v>14</v>
       </c>
       <c r="D51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,7 +1535,7 @@
         <v>14</v>
       </c>
       <c r="D52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,7 +1549,7 @@
         <v>14</v>
       </c>
       <c r="D53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1566,7 +1563,7 @@
         <v>14</v>
       </c>
       <c r="D54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1580,7 +1577,7 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1594,7 +1591,7 @@
         <v>14</v>
       </c>
       <c r="D56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1608,7 +1605,7 @@
         <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1622,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1636,7 +1633,7 @@
         <v>14</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1650,7 +1647,7 @@
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1664,7 +1661,7 @@
         <v>14</v>
       </c>
       <c r="D61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1678,7 +1675,7 @@
         <v>14</v>
       </c>
       <c r="D62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1692,7 +1689,7 @@
         <v>14</v>
       </c>
       <c r="D63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1706,7 +1703,7 @@
         <v>4</v>
       </c>
       <c r="D64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,7 +1717,7 @@
         <v>4</v>
       </c>
       <c r="D65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,7 +1731,7 @@
         <v>14</v>
       </c>
       <c r="D66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1748,7 +1745,7 @@
         <v>14</v>
       </c>
       <c r="D67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1759,10 +1756,10 @@
         <v>161</v>
       </c>
       <c r="C68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" t="s">
         <v>82</v>
-      </c>
-      <c r="D68" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1776,7 +1773,7 @@
         <v>14</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,7 +1787,7 @@
         <v>14</v>
       </c>
       <c r="D70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1801,10 +1798,10 @@
         <v>99</v>
       </c>
       <c r="C71" t="s">
+        <v>85</v>
+      </c>
+      <c r="D71" t="s">
         <v>86</v>
-      </c>
-      <c r="D71" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1818,7 +1815,7 @@
         <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1832,7 +1829,7 @@
         <v>14</v>
       </c>
       <c r="D73" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1843,10 +1840,10 @@
         <v>170</v>
       </c>
       <c r="C74" t="s">
+        <v>89</v>
+      </c>
+      <c r="D74" t="s">
         <v>90</v>
-      </c>
-      <c r="D74" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1860,7 +1857,7 @@
         <v>14</v>
       </c>
       <c r="D75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1874,7 +1871,7 @@
         <v>14</v>
       </c>
       <c r="D76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,7 +1885,7 @@
         <v>14</v>
       </c>
       <c r="D77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,7 +1899,7 @@
         <v>14</v>
       </c>
       <c r="D78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1916,7 +1913,7 @@
         <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,7 +1927,7 @@
         <v>14</v>
       </c>
       <c r="D80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1944,7 +1941,7 @@
         <v>14</v>
       </c>
       <c r="D81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1958,7 +1955,7 @@
         <v>14</v>
       </c>
       <c r="D82" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,7 +1969,7 @@
         <v>14</v>
       </c>
       <c r="D83" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,7 +1983,7 @@
         <v>14</v>
       </c>
       <c r="D84" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2000,7 +1997,7 @@
         <v>14</v>
       </c>
       <c r="D85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,7 +2011,7 @@
         <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2028,7 +2025,7 @@
         <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2042,7 +2039,7 @@
         <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2056,7 +2053,7 @@
         <v>14</v>
       </c>
       <c r="D89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2070,7 +2067,7 @@
         <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2084,7 +2081,7 @@
         <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2098,7 +2095,7 @@
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2112,7 +2109,7 @@
         <v>14</v>
       </c>
       <c r="D93" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,7 +2123,7 @@
         <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2137,10 +2134,10 @@
         <v>31</v>
       </c>
       <c r="C95" t="s">
+        <v>111</v>
+      </c>
+      <c r="D95" t="s">
         <v>112</v>
-      </c>
-      <c r="D95" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,7 +2151,7 @@
         <v>4</v>
       </c>
       <c r="D96" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2168,7 +2165,7 @@
         <v>4</v>
       </c>
       <c r="D97" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,10 +2176,10 @@
         <v>64</v>
       </c>
       <c r="C98" t="s">
+        <v>115</v>
+      </c>
+      <c r="D98" t="s">
         <v>116</v>
-      </c>
-      <c r="D98" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2196,7 +2193,7 @@
         <v>14</v>
       </c>
       <c r="D99" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2207,10 +2204,10 @@
         <v>57</v>
       </c>
       <c r="C100" t="s">
+        <v>118</v>
+      </c>
+      <c r="D100" t="s">
         <v>119</v>
-      </c>
-      <c r="D100" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,7 +2221,7 @@
         <v>4</v>
       </c>
       <c r="D101" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2238,7 +2235,7 @@
         <v>14</v>
       </c>
       <c r="D102" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2252,7 +2249,7 @@
         <v>14</v>
       </c>
       <c r="D103" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2266,7 +2263,7 @@
         <v>4</v>
       </c>
       <c r="D104" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2280,7 +2277,7 @@
         <v>14</v>
       </c>
       <c r="D105" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2294,7 +2291,7 @@
         <v>14</v>
       </c>
       <c r="D106" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2308,7 +2305,7 @@
         <v>14</v>
       </c>
       <c r="D107" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2322,7 +2319,7 @@
         <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2336,7 +2333,7 @@
         <v>4</v>
       </c>
       <c r="D109" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2350,7 +2347,7 @@
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2364,7 +2361,7 @@
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2378,7 +2375,7 @@
         <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>